<commit_message>
Programa funcional com o basico rodando e sem erros
</commit_message>
<xml_diff>
--- a/relatorio_estoque.xlsx
+++ b/relatorio_estoque.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,77 +436,77 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HOLLOW 7,5" 1,5M COM PARAFUSO</t>
+          <t>CABEÇA HOLLOW 6" COM PORTINHOLA CHAVETA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HOLLOW 6"1M COM CHAVETA</t>
+          <t>CABEÇA HOLLOW 7,5" PARAFUSO COM PORTINHOLA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CABEÇA HOLLOW 7,5 </t>
+          <t>CABEÇA HOLLOW 6" CHAVETA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CABEÇA HOLLOW 7,5" COM PORTINHOLA</t>
+          <t>CABEÇA HOLLOW 7,5" PARFUSO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CABEÇA HOLLOW 6"</t>
+          <t>HASTE HELICOIDAL 4" 1,5M</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CABEÇA HOLLOW 6" COM PORTINHOLA</t>
+          <t>HASTE HEICOIDAL 4" 1M</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HASTE HELICOIDAL 4" 1,5M</t>
+          <t>HASTE HELICOIDAL 6" 1,5M</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HASTE HELICOIDAL 4" 1M</t>
+          <t>HASTE HELICOIDAL 6" 1M</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -516,127 +516,127 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HSTE HELICOIDAL 6" 1,5M</t>
+          <t>PONTEIRA HELICOIDAL 4" 1M</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HASTE HELICOIDAL 6"  1M</t>
+          <t>PONTEIRA HELICOIDAL 6" 1,5M</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PONTEIRA HELICOIDAL 4" 1M</t>
+          <t>HASTE MACIÇA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PONTEIRA HELICOIDAL 6" 1,5M</t>
+          <t>HASTE INJEÇÃO 1,2M</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HASTE MACIÇA 42MM</t>
+          <t>HASTE INJEÇÃO 60CM</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1000</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HSTE DE INJEÇÃO 1,2M</t>
+          <t>HASTE INOX 1M</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>90</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HASTE DE INJEÇÃO 60CM</t>
+          <t>PONTEIRA FIXA INJEÇÃO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HASTE INOX 1M</t>
+          <t>PONTEIRA ARTICULADA</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PONTEIRA FIXA DE INJEÇÃO</t>
+          <t>PONTEIRA TRICONICA 4"</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PONTEIRA FIXA INOX</t>
+          <t>PONTEIRA TRICONICA 6"</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PONTEIRA DE HASTE</t>
+          <t>BATEDOR HASTE MACIÇA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PONTEIRA ARTICULADA</t>
+          <t>BATEDOR</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PONTEIRA TRICONICA 4"</t>
+          <t>SACADOR GDU</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -646,7 +646,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PONTEIRA TRICONICA 6"</t>
+          <t>PESCADOR</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -656,187 +656,187 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BATEDOR PARA HASTE MACIÇA 42MM</t>
+          <t>MINI SACADOR</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1000</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BATEDOR</t>
+          <t xml:space="preserve">SACADOR DE HASTE </t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SACADOR GDU</t>
+          <t>EXTRATOR DE HASTE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PESCADOR</t>
+          <t>GARFO HOLLOW</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MINI SACADOR</t>
+          <t>GARFO HELICOIDAL</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SACADOR DE HASTE</t>
+          <t>SACADOR DE LINER</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EXTRATOR DE HASTE</t>
+          <t>AMOSTRADOR PROBE 1,2M</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GARFO HOLLOW</t>
+          <t>AMOSTRADOR PROBE 60CM</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1000</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GARFO HELICOIDAL</t>
+          <t>MINI PROBE</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SACADOR DE LINER</t>
+          <t>MINI PROBE BI PARTIDO</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PROBE</t>
+          <t>ADAPTADOR PROBE MACHO</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PROBE 60CM</t>
+          <t>ADAPTADOR PROBE FEMEA</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MINI PROBE</t>
+          <t xml:space="preserve">PROBE BI PARTIDO </t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MINI PROBE BI PARTIDO</t>
+          <t>TE DE INJEÇÃO</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ADAPTADOR PROBE MACHO</t>
+          <t>T INOX COM SAIDA MANOMETRO</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ADAPTADOR PROBE FEMEA</t>
+          <t>CORTADOR DE LINER</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TE DE INJEÇÃO</t>
+          <t>SUPORTE DE CORTAR LINER</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>T INOX COM SAIDA MANOMETRO</t>
+          <t>BAILER DE INOX 1.1/2"</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CORTADOR DE LINER</t>
+          <t xml:space="preserve">BAILER D EINOX 3.1/4" </t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -846,61 +846,51 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SUPORTE DE CORTAR LINER</t>
+          <t>HOLLOW 6" 1M CHAVETA</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BAILER INOX 1.1/5"</t>
+          <t>HOLLOW 7,5" 1,5M COM PARAFUSO</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BAILER INOX 3.1/4"</t>
+          <t>PONTEIRA FIXA INOX</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MARTELO</t>
+          <t>BOMBA PNEUMATICA</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">HOLLOW 6"1M COM CHAVETA	</t>
+          <t>PONTEIRA HELICOIDAL 6" 1M</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>PROBE BI PARTIDO</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>368</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>